<commit_message>
uppgift 0, anonymizea name, clean data Austria
</commit_message>
<xml_diff>
--- a/Projekt_OS/Projekt_OS_2veckorsplan.xlsx
+++ b/Projekt_OS/Projekt_OS_2veckorsplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joan1\My-projects\Databehandling-Joan-Z\Projekt_OS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0CA0C02-B0EC-4D4C-82B0-71D2C7A4873D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030B935D-7A51-4B1B-BE7B-1D2311E11CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
-  <si>
-    <t>Dag</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>Aktivitet</t>
   </si>
@@ -40,63 +37,21 @@
     <t>Mån (v1)</t>
   </si>
   <si>
-    <t>Ons (v1)</t>
-  </si>
-  <si>
     <t>Fre (v1)</t>
   </si>
   <si>
     <t>Tis (v2)</t>
   </si>
   <si>
-    <t>Ons (v2)</t>
-  </si>
-  <si>
     <t>Kick-off &amp; planering</t>
   </si>
   <si>
-    <t>Ladda ner &amp; undersök data (Uppgift 0)</t>
-  </si>
-  <si>
-    <t>Landanalys (Uppgift 1)</t>
-  </si>
-  <si>
-    <t>Sportanalys (Uppgift 2)</t>
-  </si>
-  <si>
-    <t>Gemensam kodgranskning</t>
-  </si>
-  <si>
     <t>Skapa Dash-app (Uppgift 3)</t>
   </si>
   <si>
-    <t>Finputsa dashboarden</t>
-  </si>
-  <si>
-    <t>Deploya på Render.com</t>
-  </si>
-  <si>
-    <t>Förbered presentation (Uppgift 3)</t>
-  </si>
-  <si>
-    <t>Individuella videor (Uppgift 4)</t>
-  </si>
-  <si>
     <t>Alla</t>
   </si>
   <si>
-    <t>Data + Visualisering</t>
-  </si>
-  <si>
-    <t>Visualisering + Dashboard</t>
-  </si>
-  <si>
-    <t>Dashboard + Visualisering</t>
-  </si>
-  <si>
-    <t>Dashboard</t>
-  </si>
-  <si>
     <t>Presentation + Alla</t>
   </si>
   <si>
@@ -121,19 +76,40 @@
     <t>Färdig dashboard</t>
   </si>
   <si>
-    <t>Länk till deployad app</t>
-  </si>
-  <si>
     <t>Presentation klar</t>
   </si>
   <si>
-    <t>Video-länkar klara</t>
-  </si>
-  <si>
     <t>Ej påbörjad</t>
   </si>
   <si>
-    <t>Ons(v2)</t>
+    <t>Ladda ner &amp; undersök data &amp; anonymisera (Uppgift 0)</t>
+  </si>
+  <si>
+    <t>Tors (v1)</t>
+  </si>
+  <si>
+    <t>Tors(v1)</t>
+  </si>
+  <si>
+    <t>Landanalys (Uppgift 1) Data + Visualisering Moduler</t>
+  </si>
+  <si>
+    <t>Sportanalys (Uppgift 2) Data + Visualisering Moduler</t>
+  </si>
+  <si>
+    <t>Deployment Module Deploya på Render.com</t>
+  </si>
+  <si>
+    <t>Mån (v2)</t>
+  </si>
+  <si>
+    <t>Gemensam kodgranskning Förbered presentation (Uppgift 3)</t>
+  </si>
+  <si>
+    <t>Individuella videor (Uppgift 4) + presentation</t>
+  </si>
+  <si>
+    <t>Deadline</t>
   </si>
 </sst>
 </file>
@@ -501,205 +477,160 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.88671875" customWidth="1"/>
-    <col min="2" max="2" width="29.109375" customWidth="1"/>
+    <col min="2" max="2" width="52.77734375" customWidth="1"/>
     <col min="3" max="3" width="28.77734375" customWidth="1"/>
     <col min="4" max="4" width="32.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>